<commit_message>
Modification du tableau de synthèse
</commit_message>
<xml_diff>
--- a/public/Tableau de synthese.xlsx
+++ b/public/Tableau de synthese.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B8AC830-4778-460F-A75B-07EE3C3FDE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BE7A464-BBA2-4798-AEF1-145E54BA1713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t>▢ SISR</t>
   </si>
   <si>
-    <t>Adresse URL du portfolio :</t>
-  </si>
-  <si>
     <t>Compétences mises en œuvre
 Réalisations professionnelles
 (intitulé et liste des documents et productions associés)</t>
@@ -226,6 +223,9 @@
   </si>
   <si>
     <t>☑ SLAM</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : https://samuelcharbit0.github.io/samuelcharbit-portfolio/</t>
   </si>
 </sst>
 </file>
@@ -797,15 +797,48 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -841,39 +874,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1186,7 +1186,7 @@
   <dimension ref="A1:AQ82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A5" sqref="A5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1199,56 +1199,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="31"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="50" t="s">
+      <c r="A3" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="45"/>
-      <c r="H3" s="51"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="40"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="49"/>
+      <c r="A4" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="8" t="s">
         <v>4</v>
       </c>
@@ -1256,67 +1256,67 @@
         <v>5</v>
       </c>
       <c r="H4" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="52" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="41" t="s">
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="54"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="43"/>
-    </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="B6" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="C6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="42"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="13" t="s">
+      <c r="D7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="E7" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="G7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="H7" s="14" t="s">
         <v>19</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>20</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -1355,16 +1355,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
+      <c r="A8" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="44"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="46"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1403,24 +1403,24 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="26"/>
       <c r="D9" s="25"/>
       <c r="E9" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
@@ -1460,22 +1460,22 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="25"/>
       <c r="E10" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H10" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -1515,22 +1515,22 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
       <c r="E11" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" s="25"/>
       <c r="G11" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H11" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -1570,22 +1570,22 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="25"/>
       <c r="E12" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H12" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
@@ -1625,24 +1625,24 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
       <c r="E13" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H13" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I13"/>
       <c r="J13"/>
@@ -1682,26 +1682,26 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H14" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I14"/>
       <c r="J14"/>
@@ -1741,24 +1741,24 @@
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
       <c r="E15" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H15" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I15"/>
       <c r="J15"/>
@@ -1798,22 +1798,22 @@
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
       <c r="E16" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" s="25"/>
       <c r="G16" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H16" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I16"/>
       <c r="J16"/>
@@ -1853,24 +1853,24 @@
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
       <c r="E17" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H17" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I17"/>
       <c r="J17"/>
@@ -1910,28 +1910,28 @@
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G18" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H18" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I18"/>
       <c r="J18"/>
@@ -1971,24 +1971,24 @@
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="52.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="25"/>
       <c r="E19" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I19"/>
       <c r="J19"/>
@@ -2027,16 +2027,16 @@
       <c r="AQ19"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="38"/>
+      <c r="A20" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="49"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -2075,24 +2075,24 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H21" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I21"/>
       <c r="J21"/>
@@ -2132,26 +2132,26 @@
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G22" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H22" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I22"/>
       <c r="J22"/>
@@ -2191,24 +2191,24 @@
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H23" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I23"/>
       <c r="J23"/>
@@ -2239,16 +2239,16 @@
       <c r="AI23"/>
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="38"/>
+      <c r="A24" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="49"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2279,24 +2279,24 @@
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="52" t="s">
-        <v>54</v>
+        <v>37</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>53</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H25" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I25"/>
       <c r="J25"/>
@@ -2336,26 +2336,26 @@
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="52" t="s">
-        <v>53</v>
+        <v>38</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>52</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G26" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H26" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I26"/>
       <c r="J26"/>
@@ -2394,22 +2394,22 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" s="53" t="s">
-        <v>52</v>
+      <c r="A27" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>51</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E27" s="25"/>
       <c r="F27" s="10"/>
       <c r="G27" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27"/>
@@ -2973,11 +2973,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2985,6 +2980,11 @@
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -3190,15 +3190,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="b51e6d1e-8224-46a7-86ba-7d6901891049" xsi:nil="true"/>
@@ -3207,6 +3198,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3229,14 +3229,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E5CC2F8-6A3D-4E00-BE87-ABD27B2DABA8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{092602E4-9251-40C3-8AA3-A273484EC6BA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3245,4 +3237,12 @@
     <ds:schemaRef ds:uri="8955dbd3-594d-423f-94ea-9d3376d0dae5"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E5CC2F8-6A3D-4E00-BE87-ABD27B2DABA8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>